<commit_message>
fix csv import, order of unit,error columns, added STOP to be used for last row in exp file
</commit_message>
<xml_diff>
--- a/Tests/EuSorption/dbimport/Eu_on_illite.xlsx
+++ b/Tests/EuSorption/dbimport/Eu_on_illite.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeDan\OneDrive\GEMSFITS-Tutorial\Exp-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miron\git\bucket\gemsfits\GEMSFITSDEPLOY\Gemsfits1.2.1\Tests\EuSorption\dbimport\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0BB516-67C0-4064-A500-12AE2285BB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="139"/>
+    <workbookView xWindow="1670" yWindow="860" windowWidth="12930" windowHeight="7170" tabRatio="139" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOL" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -281,11 +282,14 @@
   <si>
     <t>(ml/g)</t>
   </si>
+  <si>
+    <t>STOP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
@@ -491,7 +495,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,7 +579,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -853,6 +857,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-15CB-45F6-889D-AB8EB40AA774}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1108,6 +1117,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-15CB-45F6-889D-AB8EB40AA774}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1234,7 +1248,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1514,51 +1534,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:AMH497"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12.28515625" style="1"/>
-    <col min="4" max="4" width="8.28515625" style="1"/>
-    <col min="5" max="5" width="8.5703125" style="1"/>
+    <col min="1" max="3" width="12.26953125" style="1"/>
+    <col min="4" max="4" width="8.26953125" style="1"/>
+    <col min="5" max="5" width="8.54296875" style="1"/>
     <col min="6" max="6" width="18" style="1"/>
-    <col min="7" max="9" width="15.140625" style="1"/>
+    <col min="7" max="9" width="15.1796875" style="1"/>
     <col min="10" max="10" width="7" style="1"/>
-    <col min="11" max="11" width="14.28515625" style="1"/>
-    <col min="12" max="12" width="6.85546875" style="1"/>
-    <col min="13" max="13" width="15.140625" style="1"/>
+    <col min="11" max="11" width="14.26953125" style="1"/>
+    <col min="12" max="12" width="6.81640625" style="1"/>
+    <col min="13" max="13" width="15.1796875" style="1"/>
     <col min="14" max="14" width="8" style="1"/>
     <col min="15" max="15" width="15" style="1"/>
-    <col min="16" max="16" width="6.28515625" style="1"/>
-    <col min="17" max="17" width="13.140625" style="1"/>
+    <col min="16" max="16" width="6.26953125" style="1"/>
+    <col min="17" max="17" width="13.1796875" style="1"/>
     <col min="18" max="18" width="7" style="1"/>
-    <col min="19" max="19" width="11.42578125" style="1"/>
-    <col min="20" max="20" width="6.5703125" style="1"/>
-    <col min="21" max="21" width="11.42578125" style="1"/>
-    <col min="22" max="22" width="6.7109375" style="1"/>
-    <col min="23" max="23" width="11.42578125" style="1"/>
-    <col min="24" max="24" width="5.7109375" style="1"/>
-    <col min="25" max="25" width="11.42578125" style="1"/>
-    <col min="26" max="26" width="5.5703125" style="1"/>
-    <col min="27" max="27" width="11.42578125" style="1"/>
+    <col min="19" max="19" width="11.453125" style="1"/>
+    <col min="20" max="20" width="6.54296875" style="1"/>
+    <col min="21" max="21" width="11.453125" style="1"/>
+    <col min="22" max="22" width="6.7265625" style="1"/>
+    <col min="23" max="23" width="11.453125" style="1"/>
+    <col min="24" max="24" width="5.7265625" style="1"/>
+    <col min="25" max="25" width="11.453125" style="1"/>
+    <col min="26" max="26" width="5.54296875" style="1"/>
+    <col min="27" max="27" width="11.453125" style="1"/>
     <col min="28" max="28" width="6" style="1"/>
-    <col min="29" max="29" width="16.5703125" style="1"/>
-    <col min="30" max="30" width="16.28515625" style="1"/>
+    <col min="29" max="29" width="16.54296875" style="1"/>
+    <col min="30" max="30" width="16.26953125" style="1"/>
     <col min="31" max="32" width="7" style="1"/>
-    <col min="33" max="33" width="19.140625" style="1"/>
-    <col min="34" max="268" width="12.28515625" style="1"/>
-    <col min="269" max="1023" width="8.7109375"/>
+    <col min="33" max="33" width="19.1796875" style="1"/>
+    <col min="34" max="268" width="12.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" s="2" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1022" s="2" customFormat="1" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1677,7 @@
       <c r="AMG1"/>
       <c r="AMH1"/>
     </row>
-    <row r="2" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1756,7 +1775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1854,7 +1873,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1953,7 +1972,7 @@
       </c>
       <c r="AG4"/>
     </row>
-    <row r="5" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2052,7 +2071,7 @@
       </c>
       <c r="AG5"/>
     </row>
-    <row r="6" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2151,7 +2170,7 @@
       </c>
       <c r="AG6"/>
     </row>
-    <row r="7" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2250,7 +2269,7 @@
       </c>
       <c r="AG7"/>
     </row>
-    <row r="8" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2349,7 +2368,7 @@
       </c>
       <c r="AG8"/>
     </row>
-    <row r="9" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2448,7 +2467,7 @@
       </c>
       <c r="AG9"/>
     </row>
-    <row r="10" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2547,7 +2566,7 @@
       </c>
       <c r="AG10"/>
     </row>
-    <row r="11" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2646,7 +2665,7 @@
       </c>
       <c r="AG11"/>
     </row>
-    <row r="12" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2745,7 +2764,7 @@
       </c>
       <c r="AG12"/>
     </row>
-    <row r="13" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2844,7 +2863,7 @@
       </c>
       <c r="AG13"/>
     </row>
-    <row r="14" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2943,7 +2962,7 @@
       </c>
       <c r="AG14"/>
     </row>
-    <row r="15" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3042,7 +3061,7 @@
       </c>
       <c r="AG15"/>
     </row>
-    <row r="16" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3141,7 +3160,7 @@
       </c>
       <c r="AG16"/>
     </row>
-    <row r="17" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3240,7 +3259,7 @@
       </c>
       <c r="AG17"/>
     </row>
-    <row r="18" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3339,7 +3358,7 @@
       </c>
       <c r="AG18"/>
     </row>
-    <row r="19" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3438,7 +3457,7 @@
       </c>
       <c r="AG19"/>
     </row>
-    <row r="20" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3537,7 +3556,7 @@
       </c>
       <c r="AG20"/>
     </row>
-    <row r="21" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3636,7 +3655,7 @@
       </c>
       <c r="AG21"/>
     </row>
-    <row r="22" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3735,7 +3754,7 @@
       </c>
       <c r="AG22"/>
     </row>
-    <row r="23" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3834,7 +3853,7 @@
       </c>
       <c r="AG23"/>
     </row>
-    <row r="24" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3933,7 +3952,7 @@
       </c>
       <c r="AG24"/>
     </row>
-    <row r="25" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4032,7 +4051,7 @@
       </c>
       <c r="AG25"/>
     </row>
-    <row r="26" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4131,7 +4150,7 @@
       </c>
       <c r="AG26"/>
     </row>
-    <row r="27" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4230,7 +4249,7 @@
       </c>
       <c r="AG27"/>
     </row>
-    <row r="28" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4329,7 +4348,7 @@
       </c>
       <c r="AG28"/>
     </row>
-    <row r="29" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4428,7 +4447,7 @@
       </c>
       <c r="AG29"/>
     </row>
-    <row r="30" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4527,7 +4546,7 @@
       </c>
       <c r="AG30"/>
     </row>
-    <row r="31" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4626,7 +4645,7 @@
       </c>
       <c r="AG31"/>
     </row>
-    <row r="32" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4725,7 +4744,7 @@
       </c>
       <c r="AG32"/>
     </row>
-    <row r="33" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4824,7 +4843,7 @@
       </c>
       <c r="AG33"/>
     </row>
-    <row r="34" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4923,7 +4942,7 @@
       </c>
       <c r="AG34"/>
     </row>
-    <row r="35" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5022,7 +5041,7 @@
       </c>
       <c r="AG35"/>
     </row>
-    <row r="36" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5121,7 +5140,7 @@
       </c>
       <c r="AG36"/>
     </row>
-    <row r="37" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5220,7 +5239,7 @@
       </c>
       <c r="AG37"/>
     </row>
-    <row r="38" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5319,7 +5338,7 @@
       </c>
       <c r="AG38"/>
     </row>
-    <row r="39" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5418,271 +5437,276 @@
       </c>
       <c r="AG39"/>
     </row>
-    <row r="233" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="233" ht="14.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5694,23 +5718,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" activeCellId="1" sqref="G2:H39 D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="11.5703125" style="10"/>
-    <col min="3" max="3" width="11.5703125" style="11"/>
-    <col min="4" max="5" width="11.5703125" style="12"/>
-    <col min="6" max="1025" width="10.85546875"/>
+    <col min="1" max="1" width="19.453125"/>
+    <col min="2" max="2" width="11.54296875" style="10"/>
+    <col min="3" max="3" width="11.54296875" style="11"/>
+    <col min="4" max="5" width="11.54296875" style="12"/>
+    <col min="6" max="1025" width="10.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="13" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>65</v>
       </c>
@@ -5719,7 +5743,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="21" customFormat="1" ht="20.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="17" t="s">
         <v>66</v>
       </c>
@@ -5728,7 +5752,7 @@
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" ht="21.75" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="22" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="22" t="s">
         <v>67</v>
       </c>
@@ -5737,14 +5761,14 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="24" t="s">
         <v>68</v>
       </c>
@@ -5758,7 +5782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="24"/>
       <c r="C6" s="25" t="s">
         <v>70</v>
@@ -5768,7 +5792,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="28">
         <v>2.54</v>
       </c>
@@ -5782,7 +5806,7 @@
         <v>3.3278591060743201</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="28">
         <v>2.5499999999999998</v>
       </c>
@@ -5796,7 +5820,7 @@
         <v>3.5492542280260899</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="28">
         <v>2.5499999999999998</v>
       </c>
@@ -5810,7 +5834,7 @@
         <v>3.8314696173532998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="28">
         <v>3.86</v>
       </c>
@@ -5824,7 +5848,7 @@
         <v>4.0432339535413302</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="28">
         <v>3.87</v>
       </c>
@@ -5838,7 +5862,7 @@
         <v>4.4798146572050603</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="28">
         <v>3.85</v>
       </c>
@@ -5852,7 +5876,7 @@
         <v>4.97045678805494</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="28">
         <v>4.57</v>
       </c>
@@ -5866,7 +5890,7 @@
         <v>5.2566721042950997</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="28">
         <v>4.58</v>
       </c>
@@ -5880,7 +5904,7 @@
         <v>5.4644130069207</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="28">
         <v>4.6100000000000003</v>
       </c>
@@ -5894,7 +5918,7 @@
         <v>5.3198411413054796</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="28">
         <v>5.5</v>
       </c>
@@ -5908,7 +5932,7 @@
         <v>4.4664197072638103</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="28">
         <v>5.48</v>
       </c>
@@ -5922,7 +5946,7 @@
         <v>3.5445209138374301</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="28">
         <v>5.48</v>
       </c>
@@ -5936,7 +5960,7 @@
         <v>2.2259738381402698</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="28">
         <v>5.91</v>
       </c>
@@ -5950,7 +5974,7 @@
         <v>3.3159078969593998</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="28">
         <v>5.92</v>
       </c>
@@ -5964,7 +5988,7 @@
         <v>3.5649232924940502</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="28">
         <v>5.93</v>
       </c>
@@ -5978,7 +6002,7 @@
         <v>3.8339030910813601</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="28">
         <v>6.48</v>
       </c>
@@ -5992,7 +6016,7 @@
         <v>4.0360534447880703</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="28">
         <v>6.46</v>
       </c>
@@ -6006,7 +6030,7 @@
         <v>4.4761951622904803</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="28">
         <v>6.45</v>
       </c>
@@ -6020,7 +6044,7 @@
         <v>4.9900888870914999</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="28">
         <v>6.93</v>
       </c>
@@ -6034,7 +6058,7 @@
         <v>5.2316127967580899</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="28">
         <v>6.92</v>
       </c>
@@ -6048,7 +6072,7 @@
         <v>5.3640603439114001</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="28">
         <v>6.92</v>
       </c>
@@ -6062,7 +6086,7 @@
         <v>5.3158323945131203</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="28">
         <v>7.4</v>
       </c>
@@ -6076,7 +6100,7 @@
         <v>4.4797331005251104</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="28">
         <v>7.39</v>
       </c>
@@ -6090,7 +6114,7 @@
         <v>3.5477596215579399</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="28">
         <v>7.36</v>
       </c>
@@ -6104,7 +6128,7 @@
         <v>2.2382928047602899</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="28">
         <v>7.84</v>
       </c>
@@ -6118,7 +6142,7 @@
         <v>3.3203721095653398</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="28">
         <v>7.82</v>
       </c>
@@ -6132,7 +6156,7 @@
         <v>3.5386084948610801</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="28">
         <v>7.84</v>
       </c>
@@ -6146,7 +6170,7 @@
         <v>3.8151971032606098</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="28">
         <v>8.32</v>
       </c>
@@ -6160,7 +6184,7 @@
         <v>4.0442495093656099</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="28">
         <v>8.32</v>
       </c>
@@ -6174,7 +6198,7 @@
         <v>4.4614454226635196</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="28">
         <v>8.33</v>
       </c>
@@ -6188,7 +6212,7 @@
         <v>4.9773678364172502</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="28">
         <v>8.84</v>
       </c>
@@ -6202,7 +6226,7 @@
         <v>5.1906722065273598</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="28">
         <v>8.85</v>
       </c>
@@ -6216,7 +6240,7 @@
         <v>5.4706970205926302</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="28">
         <v>9.32</v>
       </c>
@@ -6230,7 +6254,7 @@
         <v>5.2797688039989596</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="28">
         <v>9.34</v>
       </c>
@@ -6244,7 +6268,7 @@
         <v>4.4714480048803198</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="28">
         <v>9.34</v>
       </c>
@@ -6258,7 +6282,7 @@
         <v>3.5485480572389201</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="28">
         <v>10.76</v>
       </c>
@@ -6272,7 +6296,7 @@
         <v>2.2400609877178801</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="28">
         <v>10.78</v>
       </c>
@@ -6280,7 +6304,7 @@
         <v>5.4876232597531898</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="28">
         <v>10.78</v>
       </c>

</xml_diff>